<commit_message>
Carga de usuarios desde archivo de excel
</commit_message>
<xml_diff>
--- a/data/usuarios.xlsx
+++ b/data/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzagay\Documents\QA Administrador\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD6F8D0-DB23-4B74-A764-199805F8755F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECBED67-42F8-4CA9-94AD-9C6B68CC2D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F73C9C79-0F55-4E71-8BFA-77C6041FE751}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>usuario</t>
   </si>
@@ -44,36 +44,15 @@
     <t>correo</t>
   </si>
   <si>
-    <t>Martha Perales</t>
-  </si>
-  <si>
-    <t>pema1</t>
-  </si>
-  <si>
     <t>pema@gloablhitss.com</t>
   </si>
   <si>
     <t>p3r4l35#4</t>
   </si>
   <si>
-    <t>Martin Carrera</t>
-  </si>
-  <si>
-    <t>martca12</t>
-  </si>
-  <si>
-    <t>camar12@globalhits.com</t>
-  </si>
-  <si>
     <t>c4rr3ra#1</t>
   </si>
   <si>
-    <t>Jorge Castro</t>
-  </si>
-  <si>
-    <t>casjo21</t>
-  </si>
-  <si>
     <t>c45j0123</t>
   </si>
   <si>
@@ -84,6 +63,30 @@
   </si>
   <si>
     <t>perfil</t>
+  </si>
+  <si>
+    <t>Martina Flores</t>
+  </si>
+  <si>
+    <t>casjo21@gmail.com</t>
+  </si>
+  <si>
+    <t>marti1</t>
+  </si>
+  <si>
+    <t>marti1@globalhits.com</t>
+  </si>
+  <si>
+    <t>Mario Monreal</t>
+  </si>
+  <si>
+    <t>moma2</t>
+  </si>
+  <si>
+    <t>Jorge Casio</t>
+  </si>
+  <si>
+    <t>casjo86</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +483,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -489,55 +492,58 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>59</v>
@@ -547,6 +553,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{4062EE6C-138D-419F-9721-74A629D68DA8}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{A78DF1F5-60BF-4212-A2F4-44986AFE8FC5}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{EA52FEAF-633B-4953-9A69-74D94CB7CEFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>